<commit_message>
changed processData to handle subheadings - needs refinement
</commit_message>
<xml_diff>
--- a/src/Book1.xlsx
+++ b/src/Book1.xlsx
@@ -38,7 +38,7 @@
     <t>CaO2 (%)</t>
   </si>
   <si>
-    <t>MgO2 (%)</t>
+    <t>Location (deg) [Lat (deg), Long (deg)]</t>
   </si>
   <si>
     <t>this is a sub-heading to distinguish a certain thing</t>
@@ -151,7 +151,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -205,7 +205,10 @@
         <v>1.5</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1.8</v>
+        <v>45.2231</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>-121.5855</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -222,7 +225,10 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>10.5</v>
+        <v>56.2321</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>-115.2624</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,10 +250,10 @@
         <v>0.06</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>62.3</v>
+        <v>46.6262</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>4.53</v>
+        <v>-131.526</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,7 +270,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>40.2</v>
+        <v>50.223</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>-111.2605</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,7 +284,10 @@
         <v>4.8</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>10.7</v>
+        <v>60.56151</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>-98.2132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>